<commit_message>
Add Digikey part numbers
</commit_message>
<xml_diff>
--- a/BoM/BOM_TOTAL.xlsx
+++ b/BoM/BOM_TOTAL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3680F319-3BDF-45DF-8559-5B28A489B231}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BB2CD7-FA8A-4C33-83A7-D029A960CAC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="702" yWindow="702" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="103">
   <si>
     <t>Value</t>
   </si>
@@ -251,6 +251,84 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0805FT100K/RMCF0805FT100KCT-ND/1942491</t>
+  </si>
+  <si>
+    <t>PartNo</t>
+  </si>
+  <si>
+    <t>36-5005-ND</t>
+  </si>
+  <si>
+    <t>36-5006-ND</t>
+  </si>
+  <si>
+    <t>36-5007-ND</t>
+  </si>
+  <si>
+    <t>399-17617-1-ND</t>
+  </si>
+  <si>
+    <t>399-1177-1-ND</t>
+  </si>
+  <si>
+    <t>399-8039-1-ND</t>
+  </si>
+  <si>
+    <t>1276-2370-1-ND</t>
+  </si>
+  <si>
+    <t>1276-6455-1-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT3K90CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT4K70CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT33K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT39K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT100KCT-ND</t>
+  </si>
+  <si>
+    <t>TC33X-102ECT-ND</t>
+  </si>
+  <si>
+    <t>TC33X-103ECT-ND</t>
+  </si>
+  <si>
+    <t>TC33X-2-504ETR-ND</t>
+  </si>
+  <si>
+    <t>1N4148WTPMSCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF0805FT1K00CT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF0805FT10K0CT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC33X-104ECT-ND </t>
+  </si>
+  <si>
+    <t>AMAZON</t>
+  </si>
+  <si>
+    <t>INHOUSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-1336-1-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1727-6034-1-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">497-2345-1-ND </t>
   </si>
 </sst>
 </file>
@@ -579,20 +657,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="16.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="97.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="97.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,49 +684,61 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="D4">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -658,14 +748,17 @@
       <c r="D5">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -675,14 +768,17 @@
       <c r="D6">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -692,11 +788,14 @@
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -706,14 +805,17 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -723,14 +825,17 @@
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -740,14 +845,17 @@
       <c r="D10">
         <v>7</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -757,11 +865,14 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -771,11 +882,14 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -785,14 +899,17 @@
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -802,14 +919,17 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -819,14 +939,17 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -836,14 +959,17 @@
       <c r="D16">
         <v>2</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -856,11 +982,14 @@
       <c r="D17">
         <v>3</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -873,11 +1002,14 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -890,14 +1022,17 @@
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -910,25 +1045,31 @@
       <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
         <v>22</v>
       </c>
@@ -938,14 +1079,17 @@
       <c r="D22">
         <v>10</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -955,14 +1099,17 @@
       <c r="D23">
         <v>7</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>31</v>
       </c>
@@ -972,14 +1119,17 @@
       <c r="D24">
         <v>4</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
         <v>51</v>
       </c>
@@ -989,11 +1139,14 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
         <v>53</v>
       </c>
@@ -1003,11 +1156,14 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
         <v>54</v>
       </c>
@@ -1017,37 +1173,41 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E23" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E22" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E20" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E24" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E27" r:id="rId8" xr:uid="{88E7A2B3-D199-4A25-9C37-603933DE7ABA}"/>
-    <hyperlink ref="E25" r:id="rId9" xr:uid="{551884CE-00B5-4071-BFD8-E6FD6F45BFC9}"/>
-    <hyperlink ref="E26" r:id="rId10" xr:uid="{5982FC8F-F204-4CB0-B809-DC2DAF4A9096}"/>
-    <hyperlink ref="E17" r:id="rId11" xr:uid="{FD4A9A50-BF7D-4D0D-B6F5-856A5D3F71EA}"/>
-    <hyperlink ref="E18" r:id="rId12" xr:uid="{12CEF127-F057-4ED7-BF0E-099D309CAFA3}"/>
-    <hyperlink ref="E19" r:id="rId13" xr:uid="{B6A902B5-051C-4B32-9D97-8B0D98A9F220}"/>
-    <hyperlink ref="E5" r:id="rId14" xr:uid="{EEEBB18F-6C51-4BC6-A48F-25DDE0ACD569}"/>
-    <hyperlink ref="E6" r:id="rId15" xr:uid="{58F09AAA-D249-4076-81A9-80FC33E50EF3}"/>
-    <hyperlink ref="E7" r:id="rId16" xr:uid="{88E206CE-D7AB-4D48-AE57-B77F550B614D}"/>
-    <hyperlink ref="E8" r:id="rId17" xr:uid="{4371BBE4-A907-45CE-88F7-3AB4AF4BDB00}"/>
-    <hyperlink ref="E9" r:id="rId18" xr:uid="{2B60313B-0647-4FEB-A26E-F5D8B127D57F}"/>
-    <hyperlink ref="E10" r:id="rId19" xr:uid="{C4DD80B6-468E-4474-AC67-4ABDF819C0B2}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{782B186D-0B28-4F5F-AC2C-FBA14F0BB745}"/>
-    <hyperlink ref="E12" r:id="rId21" xr:uid="{E9D8747A-8D99-4020-845A-E79222FECACA}"/>
-    <hyperlink ref="E13" r:id="rId22" xr:uid="{4B8C04F2-E370-4863-ACCF-C43B1B4480B5}"/>
-    <hyperlink ref="E14" r:id="rId23" xr:uid="{BD4BE4C3-F460-4841-BDBB-CAB708466D62}"/>
-    <hyperlink ref="E15" r:id="rId24" xr:uid="{2096D76F-AC09-40CF-BF2C-A867043943DB}"/>
-    <hyperlink ref="E16" r:id="rId25" xr:uid="{D844EC71-B5EE-4401-A89D-EB11834002AF}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F22" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F24" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F27" r:id="rId6" xr:uid="{88E7A2B3-D199-4A25-9C37-603933DE7ABA}"/>
+    <hyperlink ref="F25" r:id="rId7" xr:uid="{551884CE-00B5-4071-BFD8-E6FD6F45BFC9}"/>
+    <hyperlink ref="F26" r:id="rId8" xr:uid="{5982FC8F-F204-4CB0-B809-DC2DAF4A9096}"/>
+    <hyperlink ref="F17" r:id="rId9" xr:uid="{FD4A9A50-BF7D-4D0D-B6F5-856A5D3F71EA}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{12CEF127-F057-4ED7-BF0E-099D309CAFA3}"/>
+    <hyperlink ref="F19" r:id="rId11" xr:uid="{B6A902B5-051C-4B32-9D97-8B0D98A9F220}"/>
+    <hyperlink ref="F5" r:id="rId12" xr:uid="{EEEBB18F-6C51-4BC6-A48F-25DDE0ACD569}"/>
+    <hyperlink ref="F6" r:id="rId13" xr:uid="{58F09AAA-D249-4076-81A9-80FC33E50EF3}"/>
+    <hyperlink ref="F7" r:id="rId14" xr:uid="{88E206CE-D7AB-4D48-AE57-B77F550B614D}"/>
+    <hyperlink ref="F8" r:id="rId15" xr:uid="{4371BBE4-A907-45CE-88F7-3AB4AF4BDB00}"/>
+    <hyperlink ref="F9" r:id="rId16" xr:uid="{2B60313B-0647-4FEB-A26E-F5D8B127D57F}"/>
+    <hyperlink ref="F10" r:id="rId17" xr:uid="{C4DD80B6-468E-4474-AC67-4ABDF819C0B2}"/>
+    <hyperlink ref="F11" r:id="rId18" xr:uid="{782B186D-0B28-4F5F-AC2C-FBA14F0BB745}"/>
+    <hyperlink ref="F12" r:id="rId19" xr:uid="{E9D8747A-8D99-4020-845A-E79222FECACA}"/>
+    <hyperlink ref="F13" r:id="rId20" xr:uid="{4B8C04F2-E370-4863-ACCF-C43B1B4480B5}"/>
+    <hyperlink ref="F14" r:id="rId21" xr:uid="{BD4BE4C3-F460-4841-BDBB-CAB708466D62}"/>
+    <hyperlink ref="F15" r:id="rId22" xr:uid="{2096D76F-AC09-40CF-BF2C-A867043943DB}"/>
+    <hyperlink ref="F16" r:id="rId23" xr:uid="{D844EC71-B5EE-4401-A89D-EB11834002AF}"/>
+    <hyperlink ref="F3" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F21" r:id="rId26" xr:uid="{558E24D8-803D-40D4-BB28-E0A2626C54FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>